<commit_message>
react add Map (deck.gl)
</commit_message>
<xml_diff>
--- a/students/Студенты.xlsx
+++ b/students/Студенты.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.akhpashev\dev\notes\students\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27AA05E-1DF1-4846-89CD-A605CDD10263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2ECBF21-F0C7-4AE1-B58B-E9C648C8D6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ИКС_431" sheetId="4" r:id="rId1"/>
@@ -3317,6 +3317,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="31" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -3325,24 +3336,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
@@ -3362,11 +3355,18 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="31" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -3767,8 +3767,8 @@
   <sheetPr codeName="Лист2"/>
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3792,60 +3792,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="F1" s="376" t="s">
+      <c r="F1" s="375" t="s">
         <v>274</v>
       </c>
-      <c r="G1" s="379" t="s">
+      <c r="G1" s="378" t="s">
         <v>285</v>
       </c>
-      <c r="H1" s="367" t="s">
+      <c r="H1" s="372" t="s">
         <v>286</v>
       </c>
-      <c r="I1" s="367" t="s">
+      <c r="I1" s="372" t="s">
         <v>287</v>
       </c>
-      <c r="J1" s="367" t="s">
+      <c r="J1" s="372" t="s">
         <v>281</v>
       </c>
-      <c r="K1" s="367" t="s">
+      <c r="K1" s="372" t="s">
         <v>298</v>
       </c>
-      <c r="L1" s="367" t="s">
+      <c r="L1" s="372" t="s">
         <v>282</v>
       </c>
-      <c r="M1" s="373" t="s">
+      <c r="M1" s="369" t="s">
         <v>300</v>
       </c>
-      <c r="N1" s="367" t="s">
+      <c r="N1" s="372" t="s">
         <v>283</v>
       </c>
-      <c r="O1" s="367" t="s">
+      <c r="O1" s="372" t="s">
         <v>284</v>
       </c>
-      <c r="P1" s="367" t="s">
+      <c r="P1" s="372" t="s">
         <v>288</v>
       </c>
-      <c r="Q1" s="367" t="s">
+      <c r="Q1" s="372" t="s">
         <v>289</v>
       </c>
-      <c r="R1" s="370" t="s">
+      <c r="R1" s="381" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="377"/>
-      <c r="G2" s="380"/>
-      <c r="H2" s="368"/>
-      <c r="I2" s="368"/>
-      <c r="J2" s="368"/>
-      <c r="K2" s="368"/>
-      <c r="L2" s="368"/>
-      <c r="M2" s="374"/>
-      <c r="N2" s="368"/>
-      <c r="O2" s="368"/>
-      <c r="P2" s="368"/>
-      <c r="Q2" s="368"/>
-      <c r="R2" s="371"/>
+      <c r="F2" s="376"/>
+      <c r="G2" s="379"/>
+      <c r="H2" s="373"/>
+      <c r="I2" s="373"/>
+      <c r="J2" s="373"/>
+      <c r="K2" s="373"/>
+      <c r="L2" s="373"/>
+      <c r="M2" s="370"/>
+      <c r="N2" s="373"/>
+      <c r="O2" s="373"/>
+      <c r="P2" s="373"/>
+      <c r="Q2" s="373"/>
+      <c r="R2" s="382"/>
     </row>
     <row r="3" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="220"/>
@@ -3859,19 +3859,19 @@
       <c r="E3" s="226">
         <v>7</v>
       </c>
-      <c r="F3" s="377"/>
-      <c r="G3" s="380"/>
-      <c r="H3" s="368"/>
-      <c r="I3" s="368"/>
-      <c r="J3" s="368"/>
-      <c r="K3" s="368"/>
-      <c r="L3" s="368"/>
-      <c r="M3" s="374"/>
-      <c r="N3" s="368"/>
-      <c r="O3" s="368"/>
-      <c r="P3" s="368"/>
-      <c r="Q3" s="368"/>
-      <c r="R3" s="371"/>
+      <c r="F3" s="376"/>
+      <c r="G3" s="379"/>
+      <c r="H3" s="373"/>
+      <c r="I3" s="373"/>
+      <c r="J3" s="373"/>
+      <c r="K3" s="373"/>
+      <c r="L3" s="373"/>
+      <c r="M3" s="370"/>
+      <c r="N3" s="373"/>
+      <c r="O3" s="373"/>
+      <c r="P3" s="373"/>
+      <c r="Q3" s="373"/>
+      <c r="R3" s="382"/>
     </row>
     <row r="4" spans="1:26" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="220"/>
@@ -3887,19 +3887,19 @@
       <c r="E4" s="238" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="378"/>
-      <c r="G4" s="381"/>
-      <c r="H4" s="369"/>
-      <c r="I4" s="369"/>
-      <c r="J4" s="369"/>
-      <c r="K4" s="369"/>
-      <c r="L4" s="369"/>
-      <c r="M4" s="375"/>
-      <c r="N4" s="369"/>
-      <c r="O4" s="369"/>
-      <c r="P4" s="369"/>
-      <c r="Q4" s="369"/>
-      <c r="R4" s="372"/>
+      <c r="F4" s="377"/>
+      <c r="G4" s="380"/>
+      <c r="H4" s="374"/>
+      <c r="I4" s="374"/>
+      <c r="J4" s="374"/>
+      <c r="K4" s="374"/>
+      <c r="L4" s="374"/>
+      <c r="M4" s="371"/>
+      <c r="N4" s="374"/>
+      <c r="O4" s="374"/>
+      <c r="P4" s="374"/>
+      <c r="Q4" s="374"/>
+      <c r="R4" s="383"/>
       <c r="S4" s="259" t="s">
         <v>291</v>
       </c>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="C24" s="252">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>92.5</v>
       </c>
       <c r="D24" s="249">
         <v>5</v>
@@ -4943,7 +4943,9 @@
       <c r="K24" s="290">
         <v>100</v>
       </c>
-      <c r="L24" s="230"/>
+      <c r="L24" s="290">
+        <v>100</v>
+      </c>
       <c r="M24" s="230">
         <v>1</v>
       </c>
@@ -5326,6 +5328,11 @@
     <sortCondition ref="B5:B25"/>
   </sortState>
   <mergeCells count="13">
+    <mergeCell ref="N1:N4"/>
+    <mergeCell ref="O1:O4"/>
+    <mergeCell ref="P1:P4"/>
+    <mergeCell ref="Q1:Q4"/>
+    <mergeCell ref="R1:R4"/>
     <mergeCell ref="M1:M4"/>
     <mergeCell ref="L1:L4"/>
     <mergeCell ref="F1:F4"/>
@@ -5334,11 +5341,6 @@
     <mergeCell ref="I1:I4"/>
     <mergeCell ref="J1:J4"/>
     <mergeCell ref="K1:K4"/>
-    <mergeCell ref="N1:N4"/>
-    <mergeCell ref="O1:O4"/>
-    <mergeCell ref="P1:P4"/>
-    <mergeCell ref="Q1:Q4"/>
-    <mergeCell ref="R1:R4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E6" r:id="rId1" xr:uid="{4465A7BA-0A60-4856-A192-53666DFC598C}"/>
@@ -5373,8 +5375,8 @@
   <sheetPr codeName="Лист4"/>
   <dimension ref="A1:AA59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5399,58 +5401,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="G1" s="376" t="s">
+      <c r="G1" s="375" t="s">
         <v>274</v>
       </c>
-      <c r="H1" s="379" t="s">
+      <c r="H1" s="378" t="s">
         <v>285</v>
       </c>
-      <c r="I1" s="367" t="s">
+      <c r="I1" s="372" t="s">
         <v>286</v>
       </c>
-      <c r="J1" s="367" t="s">
+      <c r="J1" s="372" t="s">
         <v>287</v>
       </c>
-      <c r="K1" s="367" t="s">
+      <c r="K1" s="372" t="s">
         <v>281</v>
       </c>
       <c r="L1" s="365"/>
-      <c r="M1" s="367" t="s">
+      <c r="M1" s="372" t="s">
         <v>282</v>
       </c>
-      <c r="N1" s="373" t="s">
+      <c r="N1" s="369" t="s">
         <v>300</v>
       </c>
-      <c r="O1" s="367" t="s">
+      <c r="O1" s="372" t="s">
         <v>283</v>
       </c>
-      <c r="P1" s="367" t="s">
+      <c r="P1" s="372" t="s">
         <v>284</v>
       </c>
-      <c r="Q1" s="367" t="s">
+      <c r="Q1" s="372" t="s">
         <v>288</v>
       </c>
-      <c r="R1" s="367" t="s">
+      <c r="R1" s="372" t="s">
         <v>289</v>
       </c>
-      <c r="S1" s="370" t="s">
+      <c r="S1" s="381" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G2" s="377"/>
-      <c r="H2" s="380"/>
-      <c r="I2" s="368"/>
-      <c r="J2" s="368"/>
-      <c r="K2" s="368"/>
+      <c r="G2" s="376"/>
+      <c r="H2" s="379"/>
+      <c r="I2" s="373"/>
+      <c r="J2" s="373"/>
+      <c r="K2" s="373"/>
       <c r="L2" s="366"/>
-      <c r="M2" s="368"/>
-      <c r="N2" s="374"/>
-      <c r="O2" s="368"/>
-      <c r="P2" s="368"/>
-      <c r="Q2" s="368"/>
-      <c r="R2" s="368"/>
-      <c r="S2" s="371"/>
+      <c r="M2" s="373"/>
+      <c r="N2" s="370"/>
+      <c r="O2" s="373"/>
+      <c r="P2" s="373"/>
+      <c r="Q2" s="373"/>
+      <c r="R2" s="373"/>
+      <c r="S2" s="382"/>
     </row>
     <row r="3" spans="1:27" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="220"/>
@@ -5465,21 +5467,21 @@
       <c r="F3" s="220">
         <v>7</v>
       </c>
-      <c r="G3" s="377"/>
-      <c r="H3" s="380"/>
-      <c r="I3" s="368"/>
-      <c r="J3" s="368"/>
-      <c r="K3" s="368"/>
-      <c r="L3" s="368" t="s">
+      <c r="G3" s="376"/>
+      <c r="H3" s="379"/>
+      <c r="I3" s="373"/>
+      <c r="J3" s="373"/>
+      <c r="K3" s="373"/>
+      <c r="L3" s="373" t="s">
         <v>298</v>
       </c>
-      <c r="M3" s="368"/>
-      <c r="N3" s="374"/>
-      <c r="O3" s="368"/>
-      <c r="P3" s="368"/>
-      <c r="Q3" s="368"/>
-      <c r="R3" s="368"/>
-      <c r="S3" s="371"/>
+      <c r="M3" s="373"/>
+      <c r="N3" s="370"/>
+      <c r="O3" s="373"/>
+      <c r="P3" s="373"/>
+      <c r="Q3" s="373"/>
+      <c r="R3" s="373"/>
+      <c r="S3" s="382"/>
     </row>
     <row r="4" spans="1:27" s="264" customFormat="1" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="263"/>
@@ -5498,19 +5500,19 @@
       <c r="F4" s="271" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="378"/>
-      <c r="H4" s="381"/>
-      <c r="I4" s="369"/>
-      <c r="J4" s="369"/>
-      <c r="K4" s="369"/>
-      <c r="L4" s="369"/>
-      <c r="M4" s="369"/>
-      <c r="N4" s="375"/>
-      <c r="O4" s="369"/>
-      <c r="P4" s="369"/>
-      <c r="Q4" s="369"/>
-      <c r="R4" s="369"/>
-      <c r="S4" s="372"/>
+      <c r="G4" s="377"/>
+      <c r="H4" s="380"/>
+      <c r="I4" s="374"/>
+      <c r="J4" s="374"/>
+      <c r="K4" s="374"/>
+      <c r="L4" s="374"/>
+      <c r="M4" s="374"/>
+      <c r="N4" s="371"/>
+      <c r="O4" s="374"/>
+      <c r="P4" s="374"/>
+      <c r="Q4" s="374"/>
+      <c r="R4" s="374"/>
+      <c r="S4" s="383"/>
       <c r="T4" s="272"/>
       <c r="U4" s="266" t="s">
         <v>291</v>
@@ -6962,21 +6964,21 @@
       <c r="F34" s="359">
         <v>45967</v>
       </c>
-      <c r="G34" s="384" t="s">
+      <c r="G34" s="368" t="s">
         <v>303</v>
       </c>
-      <c r="H34" s="383"/>
-      <c r="I34" s="383"/>
-      <c r="J34" s="383"/>
-      <c r="K34" s="383"/>
-      <c r="L34" s="383"/>
-      <c r="M34" s="383"/>
-      <c r="N34" s="383"/>
-      <c r="O34" s="383"/>
-      <c r="P34" s="383"/>
-      <c r="Q34" s="383"/>
-      <c r="R34" s="383"/>
-      <c r="S34" s="383"/>
+      <c r="H34" s="367"/>
+      <c r="I34" s="367"/>
+      <c r="J34" s="367"/>
+      <c r="K34" s="367"/>
+      <c r="L34" s="367"/>
+      <c r="M34" s="367"/>
+      <c r="N34" s="367"/>
+      <c r="O34" s="367"/>
+      <c r="P34" s="367"/>
+      <c r="Q34" s="367"/>
+      <c r="R34" s="367"/>
+      <c r="S34" s="367"/>
     </row>
     <row r="35" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="233" t="s">
@@ -7733,6 +7735,11 @@
     <sortCondition ref="B5:B29"/>
   </sortState>
   <mergeCells count="13">
+    <mergeCell ref="O1:O4"/>
+    <mergeCell ref="P1:P4"/>
+    <mergeCell ref="Q1:Q4"/>
+    <mergeCell ref="R1:R4"/>
+    <mergeCell ref="S1:S4"/>
     <mergeCell ref="N1:N4"/>
     <mergeCell ref="M1:M4"/>
     <mergeCell ref="G1:G4"/>
@@ -7741,11 +7748,6 @@
     <mergeCell ref="J1:J4"/>
     <mergeCell ref="K1:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="O1:O4"/>
-    <mergeCell ref="P1:P4"/>
-    <mergeCell ref="Q1:Q4"/>
-    <mergeCell ref="R1:R4"/>
-    <mergeCell ref="S1:S4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F11" r:id="rId1" xr:uid="{F31A88B2-28E5-46B9-8437-348D873B4C12}"/>
@@ -7785,7 +7787,7 @@
   <sheetPr codeName="Лист3"/>
   <dimension ref="A1:X44"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -7811,60 +7813,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F1" s="376" t="s">
+      <c r="F1" s="375" t="s">
         <v>274</v>
       </c>
-      <c r="G1" s="379" t="s">
+      <c r="G1" s="378" t="s">
         <v>285</v>
       </c>
-      <c r="H1" s="367" t="s">
+      <c r="H1" s="372" t="s">
         <v>286</v>
       </c>
-      <c r="I1" s="367" t="s">
+      <c r="I1" s="372" t="s">
         <v>287</v>
       </c>
-      <c r="J1" s="367" t="s">
+      <c r="J1" s="372" t="s">
         <v>281</v>
       </c>
-      <c r="K1" s="367" t="s">
+      <c r="K1" s="372" t="s">
         <v>298</v>
       </c>
-      <c r="L1" s="373" t="s">
+      <c r="L1" s="369" t="s">
         <v>300</v>
       </c>
-      <c r="M1" s="367" t="s">
+      <c r="M1" s="372" t="s">
         <v>282</v>
       </c>
-      <c r="N1" s="367" t="s">
+      <c r="N1" s="372" t="s">
         <v>283</v>
       </c>
-      <c r="O1" s="367" t="s">
+      <c r="O1" s="372" t="s">
         <v>284</v>
       </c>
-      <c r="P1" s="367" t="s">
+      <c r="P1" s="372" t="s">
         <v>288</v>
       </c>
-      <c r="Q1" s="367" t="s">
+      <c r="Q1" s="372" t="s">
         <v>289</v>
       </c>
-      <c r="R1" s="370" t="s">
+      <c r="R1" s="381" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="377"/>
-      <c r="G2" s="380"/>
-      <c r="H2" s="368"/>
-      <c r="I2" s="368"/>
-      <c r="J2" s="368"/>
-      <c r="K2" s="368"/>
-      <c r="L2" s="374"/>
-      <c r="M2" s="368"/>
-      <c r="N2" s="368"/>
-      <c r="O2" s="368"/>
-      <c r="P2" s="368"/>
-      <c r="Q2" s="368"/>
-      <c r="R2" s="371"/>
+      <c r="F2" s="376"/>
+      <c r="G2" s="379"/>
+      <c r="H2" s="373"/>
+      <c r="I2" s="373"/>
+      <c r="J2" s="373"/>
+      <c r="K2" s="373"/>
+      <c r="L2" s="370"/>
+      <c r="M2" s="373"/>
+      <c r="N2" s="373"/>
+      <c r="O2" s="373"/>
+      <c r="P2" s="373"/>
+      <c r="Q2" s="373"/>
+      <c r="R2" s="382"/>
     </row>
     <row r="3" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="220"/>
@@ -7878,19 +7880,19 @@
       <c r="E3" s="220">
         <v>7</v>
       </c>
-      <c r="F3" s="377"/>
-      <c r="G3" s="380"/>
-      <c r="H3" s="368"/>
-      <c r="I3" s="368"/>
-      <c r="J3" s="368"/>
-      <c r="K3" s="368"/>
-      <c r="L3" s="374"/>
-      <c r="M3" s="368"/>
-      <c r="N3" s="368"/>
-      <c r="O3" s="368"/>
-      <c r="P3" s="368"/>
-      <c r="Q3" s="368"/>
-      <c r="R3" s="371"/>
+      <c r="F3" s="376"/>
+      <c r="G3" s="379"/>
+      <c r="H3" s="373"/>
+      <c r="I3" s="373"/>
+      <c r="J3" s="373"/>
+      <c r="K3" s="373"/>
+      <c r="L3" s="370"/>
+      <c r="M3" s="373"/>
+      <c r="N3" s="373"/>
+      <c r="O3" s="373"/>
+      <c r="P3" s="373"/>
+      <c r="Q3" s="373"/>
+      <c r="R3" s="382"/>
     </row>
     <row r="4" spans="1:24" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="220"/>
@@ -7906,19 +7908,19 @@
       <c r="E4" s="238" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="378"/>
-      <c r="G4" s="381"/>
-      <c r="H4" s="369"/>
-      <c r="I4" s="369"/>
-      <c r="J4" s="369"/>
-      <c r="K4" s="369"/>
-      <c r="L4" s="375"/>
-      <c r="M4" s="369"/>
-      <c r="N4" s="369"/>
-      <c r="O4" s="369"/>
-      <c r="P4" s="369"/>
-      <c r="Q4" s="369"/>
-      <c r="R4" s="372"/>
+      <c r="F4" s="377"/>
+      <c r="G4" s="380"/>
+      <c r="H4" s="374"/>
+      <c r="I4" s="374"/>
+      <c r="J4" s="374"/>
+      <c r="K4" s="374"/>
+      <c r="L4" s="371"/>
+      <c r="M4" s="374"/>
+      <c r="N4" s="374"/>
+      <c r="O4" s="374"/>
+      <c r="P4" s="374"/>
+      <c r="Q4" s="374"/>
+      <c r="R4" s="383"/>
       <c r="S4" s="260" t="s">
         <v>291</v>
       </c>
@@ -9048,6 +9050,11 @@
     <sortCondition ref="B5:B20"/>
   </sortState>
   <mergeCells count="13">
+    <mergeCell ref="N1:N4"/>
+    <mergeCell ref="O1:O4"/>
+    <mergeCell ref="P1:P4"/>
+    <mergeCell ref="Q1:Q4"/>
+    <mergeCell ref="R1:R4"/>
     <mergeCell ref="M1:M4"/>
     <mergeCell ref="K1:K4"/>
     <mergeCell ref="F1:F4"/>
@@ -9056,11 +9063,6 @@
     <mergeCell ref="I1:I4"/>
     <mergeCell ref="J1:J4"/>
     <mergeCell ref="L1:L4"/>
-    <mergeCell ref="N1:N4"/>
-    <mergeCell ref="O1:O4"/>
-    <mergeCell ref="P1:P4"/>
-    <mergeCell ref="Q1:Q4"/>
-    <mergeCell ref="R1:R4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" tooltip="https://github.com/sea-krevetka/visual-prog-android" xr:uid="{593759B5-F130-422A-81CF-E366A993FDAB}"/>
@@ -9241,7 +9243,7 @@
         <f>SUM(F1:AO1)</f>
         <v>26</v>
       </c>
-      <c r="AQ1" s="382" t="s">
+      <c r="AQ1" s="384" t="s">
         <v>300</v>
       </c>
     </row>
@@ -9366,7 +9368,7 @@
       <c r="AP2" s="21" t="s">
         <v>146</v>
       </c>
-      <c r="AQ2" s="382"/>
+      <c r="AQ2" s="384"/>
       <c r="AR2" s="14" t="s">
         <v>144</v>
       </c>

</xml_diff>